<commit_message>
I found some sources we could use in matlab, or maybe in python
</commit_message>
<xml_diff>
--- a/Források.xlsx
+++ b/Források.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="48" documentId="13_ncr:1_{824E7FAD-A918-40D6-9397-0A9855B3FEAA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{DFE30461-74FB-4C3C-923E-190E5AF8E987}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{290DB7D5-9E7D-4A86-871F-547DF1AEC76D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1770" yWindow="1770" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Cím</t>
   </si>
@@ -43,23 +43,118 @@
     <t>Link</t>
   </si>
   <si>
-    <t>https://aip.scitation.org/doi/pdf/10.1063/1.4981989</t>
-  </si>
-  <si>
     <t>DRÓN</t>
   </si>
   <si>
-    <t>Drón cuccos</t>
-  </si>
-  <si>
-    <t>Drónok légellenállása</t>
+    <t>Autó pálya optimalizációja</t>
+  </si>
+  <si>
+    <t>OpenAI</t>
+  </si>
+  <si>
+    <t>From MIT 6.S094 video</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A set of high-quality implementations of reinforcement learning algorithms. Python, tensorflow  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>MAYBE can use with Matlab too</t>
+    </r>
+  </si>
+  <si>
+    <t>https://github.com/openai/baselines  With matlab: https://github.com/openai/gym/issues/239</t>
+  </si>
+  <si>
+    <t>Path Planning toolbox</t>
+  </si>
+  <si>
+    <t>There is a path planning toolbox we can use in Matlab</t>
+  </si>
+  <si>
+    <t>https://www.mathworks.com/matlabcentral/fileexchange/53739-path-planning</t>
+  </si>
+  <si>
+    <t>Optimization-Based Control</t>
+  </si>
+  <si>
+    <t>Richard M. Murray</t>
+  </si>
+  <si>
+    <t>California Institute of Technology</t>
+  </si>
+  <si>
+    <t>This problem could be solved with Optimization-based control too, but we should try the other way (AI, Neural Network..)</t>
+  </si>
+  <si>
+    <t>http://www.cds.caltech.edu/~murray/books/AM08/pdf/obc09-obc09_03Mar09.pdf</t>
+  </si>
+  <si>
+    <t>What is reinforcement learning</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=JgvyzIkgxF0</t>
+  </si>
+  <si>
+    <t>Youtube video about the reinforcment learning</t>
+  </si>
+  <si>
+    <t>Path Planning and Navigation for Autonomous Robots</t>
+  </si>
+  <si>
+    <t>Carlos Santacruz-Rosero</t>
+  </si>
+  <si>
+    <t>MathWorks</t>
+  </si>
+  <si>
+    <t>https://www.mathworks.com/videos/path-planning-and-navigation-for-autonomous-robots-1509457228757.html</t>
+  </si>
+  <si>
+    <r>
+      <t>Path planning on a created map, in matlab. This video seems useful in our case.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Model can be downloaded!</t>
+    </r>
+  </si>
+  <si>
+    <t>https://www.mathworks.com/help/driving/ref/pathplannerrrt.plan.html</t>
+  </si>
+  <si>
+    <t>Oszlop1</t>
+  </si>
+  <si>
+    <t>Matlab path planning on more complex maps</t>
+  </si>
+  <si>
+    <t>https://www.mathworks.com/help/robotics/examples/path-planning-in-environments-of-difference-complexity.html</t>
+  </si>
+  <si>
+    <t>Path Planning in Environments of Different Complexity</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -104,6 +199,14 @@
       <b/>
       <sz val="13"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
@@ -205,11 +308,11 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -270,14 +373,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CC8358EE-13DA-44DD-8F82-A99BBDCE6A04}" name="Táblázat1" displayName="Táblázat1" ref="C2:G19" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1" tableBorderDxfId="0">
-  <autoFilter ref="C2:G19" xr:uid="{5805CB28-0203-435C-B94B-3F9DE81A537C}"/>
-  <tableColumns count="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CC8358EE-13DA-44DD-8F82-A99BBDCE6A04}" name="Táblázat1" displayName="Táblázat1" ref="C2:H19" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1" tableBorderDxfId="0">
+  <autoFilter ref="C2:H19" xr:uid="{5805CB28-0203-435C-B94B-3F9DE81A537C}"/>
+  <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{A642602D-D5A1-475C-B96E-4AB1E9438564}" name="Cím"/>
     <tableColumn id="2" xr3:uid="{BF169805-D4CC-47BE-9598-F1C592797089}" name="Szerző"/>
     <tableColumn id="3" xr3:uid="{D52D71C2-EDC6-4092-8D42-BA4EA12FA8E3}" name="Egyetem / Kutatóközpont"/>
     <tableColumn id="4" xr3:uid="{1220319E-5A5F-4522-AF9F-E52CD06EFED9}" name="Összefoglaló"/>
     <tableColumn id="5" xr3:uid="{B60EACBB-B52F-4779-9FBB-2E6D7ADFF73B}" name="Link"/>
+    <tableColumn id="6" xr3:uid="{605F0A8D-40B8-4BE5-B144-3A3E474F37C8}" name="Oszlop1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -546,10 +650,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C1:G26"/>
+  <dimension ref="C1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -561,16 +665,16 @@
     <col min="7" max="7" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:7" ht="53.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C1" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-    </row>
-    <row r="2" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="3:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C1" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+    </row>
+    <row r="2" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C2" s="2" t="s">
         <v>0</v>
       </c>
@@ -586,69 +690,125 @@
       <c r="G2" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C3" s="8" t="s">
+      <c r="H2" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="3:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="C3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C4" s="4"/>
+      <c r="F3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="3:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="C4" s="4" t="s">
+        <v>11</v>
+      </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="5"/>
-    </row>
-    <row r="5" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="5"/>
-    </row>
-    <row r="6" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C6" s="4"/>
+      <c r="F4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="3:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="C5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="3:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="C6" s="4" t="s">
+        <v>19</v>
+      </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="5"/>
-    </row>
-    <row r="7" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="5"/>
-    </row>
-    <row r="8" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C8" s="4"/>
+      <c r="F6" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="3:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="C7" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="3:8" ht="105" x14ac:dyDescent="0.25">
+      <c r="C8" s="4" t="s">
+        <v>31</v>
+      </c>
       <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="5"/>
-    </row>
-    <row r="9" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="F8" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="3:8" x14ac:dyDescent="0.25">
       <c r="G9" s="6"/>
     </row>
     <row r="26" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="C1:G1"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="G3" r:id="rId1" display="https://github.com/openai/baselines" xr:uid="{489912AD-0113-4B94-A41F-7FBD82807D7B}"/>
+    <hyperlink ref="G4" r:id="rId2" xr:uid="{ED24BC6E-2EF1-4AA0-BDEA-3A5E7E3EF776}"/>
+    <hyperlink ref="G5" r:id="rId3" xr:uid="{273AB6FD-D784-49A5-B6EF-0FE66A93A28B}"/>
+    <hyperlink ref="G6" r:id="rId4" xr:uid="{665BD3D5-01E2-4AE3-8E70-575EE637A314}"/>
+    <hyperlink ref="G7" r:id="rId5" xr:uid="{4C1D6D9A-64BE-438F-B2A2-A6BCCA81B761}"/>
+    <hyperlink ref="H7" r:id="rId6" xr:uid="{8B2E289F-694C-4478-AE2E-E49F50015DC0}"/>
+    <hyperlink ref="G8" r:id="rId7" xr:uid="{3EDF5A96-0B50-4690-B5F0-E6FDBD060036}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId8"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId9"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Small update to one of the referals
</commit_message>
<xml_diff>
--- a/Források.xlsx
+++ b/Források.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{290DB7D5-9E7D-4A86-871F-547DF1AEC76D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEB5F482-7450-47D3-9CB3-F92C1573152E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1770" yWindow="1770" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -141,13 +141,13 @@
     <t>Oszlop1</t>
   </si>
   <si>
-    <t>Matlab path planning on more complex maps</t>
-  </si>
-  <si>
     <t>https://www.mathworks.com/help/robotics/examples/path-planning-in-environments-of-difference-complexity.html</t>
   </si>
   <si>
     <t>Path Planning in Environments of Different Complexity</t>
+  </si>
+  <si>
+    <t>Matlab path planning on more complex maps. (I think the last AES laboratory we made a map like this from an image!)</t>
   </si>
 </sst>
 </file>
@@ -653,7 +653,7 @@
   <dimension ref="C1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -774,14 +774,14 @@
     </row>
     <row r="8" spans="3:8" ht="105" x14ac:dyDescent="0.25">
       <c r="C8" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D8" s="4"/>
       <c r="F8" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G8" s="5" t="s">
         <v>29</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="9" spans="3:8" x14ac:dyDescent="0.25">

</xml_diff>